<commit_message>
update test data and reports
</commit_message>
<xml_diff>
--- a/Local/Data/Export/DQ-Report_dqTestData_2020.xlsx
+++ b/Local/Data/Export/DQ-Report_dqTestData_2020.xlsx
@@ -352,7 +352,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -814,13 +814,6 @@
         </is>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Folgende mandatorische Items fehlen:  PLZ , Land , Kontakt_Klasse , Fall_Status , DiagnoseRolle , Diagnosedatum</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -828,7 +821,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:AA2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -847,12 +840,12 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>missing_item_rate</t>
+          <t>item_completeness_rate</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>missing_value_rate</t>
+          <t>value_completeness_rate</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -862,7 +855,7 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>outlier_rate</t>
+          <t>range_plausibility_rate</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -877,42 +870,97 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>duplication_rate</t>
+          <t>rdCase_dissimilarity_rate</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
+          <t>rdCase_rel_py_ipat</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>tracerCase_rel_py_ipat</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>unambigous_rdCase_rel_py_ipat</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>orphaCase_rel_py_ipat</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
           <t>orphaCoding_no_py</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>tracerCase_no_py</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>orphaCase_no_py</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>unambigous_rdCase_no_py</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>rdCase_no_py</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>case_no_py</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>patient_no_py</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>case_no_py_ipat</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>orphaMissing_no_py</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>implausible_codeLink_no_py</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>missing_item_no_py</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>missing_value_no_py</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>outlier_no_py</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>duplicateCase_no_py</t>
         </is>
       </c>
     </row>
@@ -926,16 +974,16 @@
         <v>2020</v>
       </c>
       <c r="C2">
-        <v>42.86</v>
+        <v>100</v>
       </c>
       <c r="D2">
-        <v>2.36</v>
+        <v>59.51</v>
       </c>
       <c r="E2">
         <v>50</v>
       </c>
       <c r="F2">
-        <v>6.41</v>
+        <v>93.75</v>
       </c>
       <c r="G2">
         <v>33.33</v>
@@ -944,28 +992,61 @@
         <v>41.18</v>
       </c>
       <c r="I2">
-        <v>3.7</v>
+        <v>96.3</v>
       </c>
       <c r="J2">
+        <v>0.17</v>
+      </c>
+      <c r="K2">
+        <v>0.04</v>
+      </c>
+      <c r="L2">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="M2">
+        <v>0.15</v>
+      </c>
+      <c r="N2">
         <v>15</v>
       </c>
-      <c r="K2">
+      <c r="O2">
+        <v>4</v>
+      </c>
+      <c r="P2">
         <v>15</v>
       </c>
-      <c r="L2">
+      <c r="Q2">
         <v>7</v>
       </c>
-      <c r="M2">
+      <c r="R2">
         <v>17</v>
       </c>
-      <c r="N2">
+      <c r="S2">
         <v>26</v>
       </c>
-      <c r="O2">
+      <c r="T2">
         <v>25</v>
       </c>
-      <c r="P2">
+      <c r="U2">
         <v>10000</v>
+      </c>
+      <c r="V2">
+        <v>2</v>
+      </c>
+      <c r="W2">
+        <v>10</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>5</v>
+      </c>
+      <c r="AA2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update readme and reports
</commit_message>
<xml_diff>
--- a/Local/Data/Export/DQ-Report_dqTestData_2020.xlsx
+++ b/Local/Data/Export/DQ-Report_dqTestData_2020.xlsx
@@ -821,7 +821,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -840,12 +840,12 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>item_completeness_rate</t>
+          <t>missing_item_rate</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>value_completeness_rate</t>
+          <t>missing_value_rate</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -855,7 +855,7 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>range_plausibility_rate</t>
+          <t>outlier_rate</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -870,97 +870,57 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>rdCase_dissimilarity_rate</t>
+          <t>duplication_rate</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>rdCase_rel_py_ipat</t>
+          <t>tracerCase_rel_py_ipat</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>tracerCase_rel_py_ipat</t>
+          <t>unambigous_rdCase_rel_py_ipat</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>unambigous_rdCase_rel_py_ipat</t>
+          <t>orphaCase_rel_py_ipat</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>orphaCase_rel_py_ipat</t>
+          <t>orphaCoding_no_py</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>orphaCoding_no_py</t>
+          <t>orphaCase_no_py</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>tracerCase_no_py</t>
+          <t>unambigous_rdCase_no_py</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>orphaCase_no_py</t>
+          <t>rdCase_no_py</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>unambigous_rdCase_no_py</t>
+          <t>case_no_py</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>rdCase_no_py</t>
+          <t>patient_no_py</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>case_no_py</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>patient_no_py</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
           <t>case_no_py_ipat</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>orphaMissing_no_py</t>
-        </is>
-      </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>implausible_codeLink_no_py</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>missing_item_no_py</t>
-        </is>
-      </c>
-      <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t>missing_value_no_py</t>
-        </is>
-      </c>
-      <c r="Z1" s="1" t="inlineStr">
-        <is>
-          <t>outlier_no_py</t>
-        </is>
-      </c>
-      <c r="AA1" s="1" t="inlineStr">
-        <is>
-          <t>duplicateCase_no_py</t>
         </is>
       </c>
     </row>
@@ -974,16 +934,16 @@
         <v>2020</v>
       </c>
       <c r="C2">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>59.51</v>
+        <v>40.49</v>
       </c>
       <c r="E2">
         <v>50</v>
       </c>
       <c r="F2">
-        <v>93.75</v>
+        <v>6.25</v>
       </c>
       <c r="G2">
         <v>33.33</v>
@@ -992,61 +952,37 @@
         <v>41.18</v>
       </c>
       <c r="I2">
-        <v>96.3</v>
+        <v>3.7</v>
       </c>
       <c r="J2">
-        <v>0.17</v>
+        <v>0.04</v>
       </c>
       <c r="K2">
-        <v>0.04</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="L2">
-        <v>0.07000000000000001</v>
+        <v>0.15</v>
       </c>
       <c r="M2">
-        <v>0.15</v>
+        <v>15</v>
       </c>
       <c r="N2">
         <v>15</v>
       </c>
       <c r="O2">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="P2">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="Q2">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="R2">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="S2">
-        <v>26</v>
-      </c>
-      <c r="T2">
-        <v>25</v>
-      </c>
-      <c r="U2">
         <v>10000</v>
-      </c>
-      <c r="V2">
-        <v>2</v>
-      </c>
-      <c r="W2">
-        <v>10</v>
-      </c>
-      <c r="X2">
-        <v>0</v>
-      </c>
-      <c r="Y2">
-        <v>0</v>
-      </c>
-      <c r="Z2">
-        <v>5</v>
-      </c>
-      <c r="AA2">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>